<commit_message>
digest map plot and massacre output support added
</commit_message>
<xml_diff>
--- a/pytheas_data/MS_1_2_charges.xlsx
+++ b/pytheas_data/MS_1_2_charges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrwill/prog/pytheas_tk_interface/pytheas_dev/pytheas_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrwill/prog/Pytheas_Folder/Pytheas_Qt_root/Pytheas_Qt/pytheas_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4982571-20D1-1248-9FEC-66CD14CF5375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A76BDD-C09F-3A4E-89CC-02AED73A30D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="760" windowWidth="28580" windowHeight="18360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>Charges</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8</t>
   </si>
 </sst>
 </file>
@@ -1092,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1263,6 +1266,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>